<commit_message>
WIP: Combine SMART and Full EHR requirements in spreadsheet
</commit_message>
<xml_diff>
--- a/lib/davinci_dtr_test_kit/requirements/hl7.fhir.us.davinci-dtr_2.0.1_requirements.xlsx
+++ b/lib/davinci_dtr_test_kit/requirements/hl7.fhir.us.davinci-dtr_2.0.1_requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstrassner/repo/inferno/davinci-dtr-test-kit/lib/davinci_dtr_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9434586-F2F9-BB49-8DA8-12646045E0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888744AD-FC0D-F24B-A54A-9CA699BF4E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1700" windowWidth="43120" windowHeight="24360" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
+    <workbookView xWindow="3060" yWindow="2860" windowWidth="43120" windowHeight="24360" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="9" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1994" uniqueCount="614">
   <si>
     <r>
       <rPr>
@@ -1957,15 +1957,6 @@
   </si>
   <si>
     <t>https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-dtr-smart-client.html#behavior</t>
-  </si>
-  <si>
-    <t>[SMART Clients] **SHALL** support the [`$questionnaire-package`](http://hl7.org/fhir/us/davinci-dtr/OperationDefinition/questionnaire-package) operation.</t>
-  </si>
-  <si>
-    <t>[SMART Clients] **SHALL** support the [`$expand`]http://hl7.org/fhir/OperationDefinition/ValueSet-expand) operation.</t>
-  </si>
-  <si>
-    <t>[SMART Clients] **SHALL** support the [`$next-question`](http://hl7.org/fhir/uv/sdc/OperationDefinition/Questionnaire-next-question) operation.</t>
   </si>
   <si>
     <t>https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-dtr-smart-client.html</t>
@@ -3242,6 +3233,24 @@
   </si>
   <si>
     <t>Actors*</t>
+  </si>
+  <si>
+    <t>[Full EHR, SMART Clients] **SHALL** support the [`$questionnaire-package`](http://hl7.org/fhir/us/davinci-dtr/OperationDefinition/questionnaire-package) operation.</t>
+  </si>
+  <si>
+    <t>[Full EHR, SMART Clients] **SHALL** support the [`$expand`]http://hl7.org/fhir/OperationDefinition/ValueSet-expand) operation.</t>
+  </si>
+  <si>
+    <t>[Full EHR, SMART Clients] **SHALL** support the [`$next-question`](http://hl7.org/fhir/uv/sdc/OperationDefinition/Questionnaire-next-question) operation.</t>
+  </si>
+  <si>
+    <t>DEPRECATED - merged with corresponding SMART Client requirement (242)</t>
+  </si>
+  <si>
+    <t>DEPRECATED - merged with corresponding SMART Client requirement (243)</t>
+  </si>
+  <si>
+    <t>DEPRECATED - merged with corresponding SMART Client requirement (244)</t>
   </si>
 </sst>
 </file>
@@ -4118,7 +4127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6AA7094-ECFF-0B4E-A5C9-6F41B8D76EEB}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4150,7 +4159,7 @@
     </row>
     <row r="4" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="44" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="36"/>
@@ -4203,11 +4212,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0272D98A-080C-3945-A7E0-CB54FB3A65A9}">
   <dimension ref="A1:AC476"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="8" ySplit="1" topLeftCell="L238" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B242" sqref="B242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4224,7 +4233,8 @@
     <col min="10" max="10" width="22" style="30" customWidth="1"/>
     <col min="11" max="11" width="10.5" style="30" customWidth="1"/>
     <col min="12" max="12" width="25.83203125" style="30" customWidth="1"/>
-    <col min="13" max="14" width="25.83203125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="38.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.83203125" style="9" customWidth="1"/>
     <col min="15" max="15" width="20" style="10" customWidth="1"/>
     <col min="16" max="16" width="28.5" style="10" customWidth="1"/>
     <col min="17" max="17" width="10.83203125" style="16"/>
@@ -4252,7 +4262,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>11</v>
@@ -5429,7 +5439,7 @@
         <v>63</v>
       </c>
       <c r="T31" s="16" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="102" x14ac:dyDescent="0.2">
@@ -5472,7 +5482,7 @@
         <v>configuring-appehr-to-payer-connectivity</v>
       </c>
       <c r="T32" s="16" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="119" x14ac:dyDescent="0.2">
@@ -6633,7 +6643,7 @@
         <v>131</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>28</v>
@@ -6718,7 +6728,7 @@
         <v>133</v>
       </c>
       <c r="T70" s="16" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="71" spans="1:20" ht="51" x14ac:dyDescent="0.2">
@@ -6752,7 +6762,7 @@
         <v>133</v>
       </c>
       <c r="T71" s="16" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="72" spans="1:20" ht="170" x14ac:dyDescent="0.2">
@@ -12085,13 +12095,13 @@
         <v>397</v>
       </c>
       <c r="C242" s="8" t="s">
-        <v>398</v>
+        <v>608</v>
       </c>
       <c r="D242" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E242" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G242" s="7" t="b">
         <v>0</v>
@@ -12113,13 +12123,13 @@
         <v>397</v>
       </c>
       <c r="C243" s="8" t="s">
-        <v>399</v>
+        <v>609</v>
       </c>
       <c r="D243" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E243" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G243" s="7" t="b">
         <v>0</v>
@@ -12133,7 +12143,7 @@
         <v>behavior</v>
       </c>
     </row>
-    <row r="244" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A244" s="7">
         <v>244</v>
       </c>
@@ -12141,13 +12151,13 @@
         <v>397</v>
       </c>
       <c r="C244" s="8" t="s">
-        <v>400</v>
+        <v>610</v>
       </c>
       <c r="D244" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E244" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G244" s="7" t="b">
         <v>0</v>
@@ -12166,10 +12176,10 @@
         <v>245</v>
       </c>
       <c r="B245" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C245" s="8" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D245" s="7" t="s">
         <v>28</v>
@@ -12194,10 +12204,10 @@
         <v>246</v>
       </c>
       <c r="B246" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C246" s="8" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D246" s="7" t="s">
         <v>28</v>
@@ -12222,10 +12232,10 @@
         <v>247</v>
       </c>
       <c r="B247" s="11" t="s">
+        <v>398</v>
+      </c>
+      <c r="C247" s="8" t="s">
         <v>401</v>
-      </c>
-      <c r="C247" s="8" t="s">
-        <v>404</v>
       </c>
       <c r="D247" s="7" t="s">
         <v>28</v>
@@ -12250,10 +12260,10 @@
         <v>248</v>
       </c>
       <c r="B248" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C248" s="8" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D248" s="7" t="s">
         <v>28</v>
@@ -12278,10 +12288,10 @@
         <v>249</v>
       </c>
       <c r="B249" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C249" s="8" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D249" s="7" t="s">
         <v>28</v>
@@ -12306,10 +12316,10 @@
         <v>250</v>
       </c>
       <c r="B250" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C250" s="8" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D250" s="7" t="s">
         <v>28</v>
@@ -12334,10 +12344,10 @@
         <v>251</v>
       </c>
       <c r="B251" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C251" s="8" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D251" s="7" t="s">
         <v>28</v>
@@ -12362,10 +12372,10 @@
         <v>252</v>
       </c>
       <c r="B252" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C252" s="8" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D252" s="7" t="s">
         <v>28</v>
@@ -12390,10 +12400,10 @@
         <v>253</v>
       </c>
       <c r="B253" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C253" s="8" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D253" s="7" t="s">
         <v>28</v>
@@ -12418,10 +12428,10 @@
         <v>254</v>
       </c>
       <c r="B254" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C254" s="8" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D254" s="7" t="s">
         <v>28</v>
@@ -12446,10 +12456,10 @@
         <v>255</v>
       </c>
       <c r="B255" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C255" s="8" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D255" s="7" t="s">
         <v>28</v>
@@ -12474,10 +12484,10 @@
         <v>256</v>
       </c>
       <c r="B256" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C256" s="8" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D256" s="7" t="s">
         <v>28</v>
@@ -12502,10 +12512,10 @@
         <v>257</v>
       </c>
       <c r="B257" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C257" s="8" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D257" s="7" t="s">
         <v>28</v>
@@ -12530,10 +12540,10 @@
         <v>258</v>
       </c>
       <c r="B258" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C258" s="8" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D258" s="7" t="s">
         <v>28</v>
@@ -12558,10 +12568,10 @@
         <v>259</v>
       </c>
       <c r="B259" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C259" s="8" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D259" s="7" t="s">
         <v>28</v>
@@ -12586,10 +12596,10 @@
         <v>260</v>
       </c>
       <c r="B260" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C260" s="8" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D260" s="7" t="s">
         <v>28</v>
@@ -12614,10 +12624,10 @@
         <v>261</v>
       </c>
       <c r="B261" s="11" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C261" s="8" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D261" s="7" t="s">
         <v>28</v>
@@ -12642,10 +12652,10 @@
         <v>262</v>
       </c>
       <c r="B262" s="11" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C262" s="8" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D262" s="7" t="s">
         <v>28</v>
@@ -12664,16 +12674,19 @@
         <f t="array" ref="N262">SECTION_NAME(B262)</f>
         <v>behavior</v>
       </c>
+      <c r="T262" s="16" t="s">
+        <v>611</v>
+      </c>
     </row>
     <row r="263" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A263" s="7">
         <v>263</v>
       </c>
       <c r="B263" s="11" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C263" s="8" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D263" s="7" t="s">
         <v>28</v>
@@ -12692,16 +12705,19 @@
         <f t="array" ref="N263">SECTION_NAME(B263)</f>
         <v>behavior</v>
       </c>
+      <c r="T263" s="16" t="s">
+        <v>612</v>
+      </c>
     </row>
     <row r="264" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A264" s="7">
         <v>264</v>
       </c>
       <c r="B264" s="11" t="s">
+        <v>416</v>
+      </c>
+      <c r="C264" s="8" t="s">
         <v>419</v>
-      </c>
-      <c r="C264" s="8" t="s">
-        <v>422</v>
       </c>
       <c r="D264" s="7" t="s">
         <v>28</v>
@@ -12720,16 +12736,19 @@
         <f t="array" ref="N264">SECTION_NAME(B264)</f>
         <v>behavior</v>
       </c>
+      <c r="T264" s="16" t="s">
+        <v>613</v>
+      </c>
     </row>
     <row r="265" spans="1:20" ht="68" x14ac:dyDescent="0.2">
       <c r="A265" s="7">
         <v>265</v>
       </c>
       <c r="B265" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C265" s="8" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D265" s="7" t="s">
         <v>28</v>
@@ -12755,7 +12774,7 @@
         <v/>
       </c>
       <c r="T265" s="16" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="266" spans="1:20" ht="68" x14ac:dyDescent="0.2">
@@ -12763,10 +12782,10 @@
         <v>266</v>
       </c>
       <c r="B266" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="C266" s="8" t="s">
         <v>423</v>
-      </c>
-      <c r="C266" s="8" t="s">
-        <v>426</v>
       </c>
       <c r="D266" s="7" t="s">
         <v>28</v>
@@ -12792,7 +12811,7 @@
         <v/>
       </c>
       <c r="T266" s="16" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="267" spans="1:20" ht="68" x14ac:dyDescent="0.2">
@@ -12800,10 +12819,10 @@
         <v>267</v>
       </c>
       <c r="B267" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C267" s="8" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D267" s="7" t="s">
         <v>28</v>
@@ -12829,7 +12848,7 @@
         <v/>
       </c>
       <c r="T267" s="16" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="268" spans="1:20" ht="68" x14ac:dyDescent="0.2">
@@ -12837,10 +12856,10 @@
         <v>268</v>
       </c>
       <c r="B268" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C268" s="8" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D268" s="7" t="s">
         <v>28</v>
@@ -12866,7 +12885,7 @@
         <v/>
       </c>
       <c r="T268" s="16" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="269" spans="1:20" ht="68" x14ac:dyDescent="0.2">
@@ -12874,10 +12893,10 @@
         <v>269</v>
       </c>
       <c r="B269" s="11" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C269" s="8" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D269" s="7" t="s">
         <v>28</v>
@@ -12903,7 +12922,7 @@
         <v/>
       </c>
       <c r="T269" s="16" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="270" spans="1:20" ht="68" x14ac:dyDescent="0.2">
@@ -12911,10 +12930,10 @@
         <v>270</v>
       </c>
       <c r="B270" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C270" s="8" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D270" s="7" t="s">
         <v>28</v>
@@ -12940,7 +12959,7 @@
         <v/>
       </c>
       <c r="T270" s="16" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="271" spans="1:20" ht="34" x14ac:dyDescent="0.2">
@@ -12948,10 +12967,10 @@
         <v>271</v>
       </c>
       <c r="B271" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C271" s="8" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D271" s="7" t="s">
         <v>52</v>
@@ -12982,10 +13001,10 @@
         <v>272</v>
       </c>
       <c r="B272" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C272" s="8" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D272" s="7" t="s">
         <v>52</v>
@@ -13016,10 +13035,10 @@
         <v>273</v>
       </c>
       <c r="B273" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C273" s="8" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D273" s="7" t="s">
         <v>52</v>
@@ -13050,10 +13069,10 @@
         <v>274</v>
       </c>
       <c r="B274" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C274" s="8" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D274" s="7" t="s">
         <v>52</v>
@@ -13084,10 +13103,10 @@
         <v>275</v>
       </c>
       <c r="B275" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C275" s="8" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D275" s="7" t="s">
         <v>52</v>
@@ -13118,10 +13137,10 @@
         <v>276</v>
       </c>
       <c r="B276" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C276" s="8" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D276" s="7" t="s">
         <v>52</v>
@@ -13152,10 +13171,10 @@
         <v>277</v>
       </c>
       <c r="B277" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C277" s="8" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D277" s="7" t="s">
         <v>52</v>
@@ -13186,10 +13205,10 @@
         <v>278</v>
       </c>
       <c r="B278" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C278" s="8" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D278" s="7" t="s">
         <v>52</v>
@@ -13220,10 +13239,10 @@
         <v>279</v>
       </c>
       <c r="B279" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C279" s="8" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D279" s="7" t="s">
         <v>52</v>
@@ -13254,10 +13273,10 @@
         <v>280</v>
       </c>
       <c r="B280" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C280" s="8" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D280" s="7" t="s">
         <v>52</v>
@@ -13288,10 +13307,10 @@
         <v>281</v>
       </c>
       <c r="B281" s="7" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C281" s="8" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D281" s="7" t="s">
         <v>28</v>
@@ -13322,10 +13341,10 @@
         <v>282</v>
       </c>
       <c r="B282" s="11" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C282" s="8" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D282" s="7" t="s">
         <v>52</v>
@@ -13350,10 +13369,10 @@
         <v>283</v>
       </c>
       <c r="B283" s="7" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C283" s="8" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D283" s="7" t="s">
         <v>52</v>
@@ -13378,10 +13397,10 @@
         <v>284</v>
       </c>
       <c r="B284" s="11" t="s">
+        <v>439</v>
+      </c>
+      <c r="C284" s="8" t="s">
         <v>442</v>
-      </c>
-      <c r="C284" s="8" t="s">
-        <v>445</v>
       </c>
       <c r="D284" s="7" t="s">
         <v>28</v>
@@ -13406,10 +13425,10 @@
         <v>285</v>
       </c>
       <c r="B285" s="11" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C285" s="8" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D285" s="7" t="s">
         <v>28</v>
@@ -13434,10 +13453,10 @@
         <v>286</v>
       </c>
       <c r="B286" s="7" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C286" s="8" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D286" s="7" t="s">
         <v>52</v>
@@ -13462,10 +13481,10 @@
         <v>287</v>
       </c>
       <c r="B287" s="7" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C287" s="8" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D287" s="7" t="s">
         <v>52</v>
@@ -13490,10 +13509,10 @@
         <v>288</v>
       </c>
       <c r="B288" s="7" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C288" s="8" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D288" s="7" t="s">
         <v>52</v>
@@ -13518,10 +13537,10 @@
         <v>289</v>
       </c>
       <c r="B289" s="7" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C289" s="8" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D289" s="7" t="s">
         <v>52</v>
@@ -13546,10 +13565,10 @@
         <v>290</v>
       </c>
       <c r="B290" s="11" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C290" s="8" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D290" s="7" t="s">
         <v>104</v>
@@ -13574,10 +13593,10 @@
         <v>291</v>
       </c>
       <c r="B291" s="7" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C291" s="8" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D291" s="7" t="s">
         <v>52</v>
@@ -13602,10 +13621,10 @@
         <v>292</v>
       </c>
       <c r="B292" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C292" s="8" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D292" s="7" t="s">
         <v>28</v>
@@ -13630,10 +13649,10 @@
         <v>293</v>
       </c>
       <c r="B293" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C293" s="8" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D293" s="7" t="s">
         <v>28</v>
@@ -13658,10 +13677,10 @@
         <v>294</v>
       </c>
       <c r="B294" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="C294" s="8" t="s">
         <v>453</v>
-      </c>
-      <c r="C294" s="8" t="s">
-        <v>456</v>
       </c>
       <c r="D294" s="7" t="s">
         <v>28</v>
@@ -13686,10 +13705,10 @@
         <v>295</v>
       </c>
       <c r="B295" s="11" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C295" s="8" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D295" s="7" t="s">
         <v>28</v>
@@ -13714,10 +13733,10 @@
         <v>296</v>
       </c>
       <c r="B296" s="11" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C296" s="8" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D296" s="7" t="s">
         <v>28</v>
@@ -13742,10 +13761,10 @@
         <v>297</v>
       </c>
       <c r="B297" s="11" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C297" s="8" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D297" s="7" t="s">
         <v>28</v>
@@ -13770,10 +13789,10 @@
         <v>298</v>
       </c>
       <c r="B298" s="11" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C298" s="8" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D298" s="7" t="s">
         <v>28</v>
@@ -13798,10 +13817,10 @@
         <v>299</v>
       </c>
       <c r="B299" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C299" s="8" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D299" s="7" t="s">
         <v>28</v>
@@ -13826,10 +13845,10 @@
         <v>300</v>
       </c>
       <c r="B300" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C300" s="8" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D300" s="7" t="s">
         <v>28</v>
@@ -13841,7 +13860,7 @@
         <v>1</v>
       </c>
       <c r="H300" s="16" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="M300" s="9" t="str" cm="1">
         <f t="array" ref="M300">PAGE_NAME(B300)</f>
@@ -13857,10 +13876,10 @@
         <v>301</v>
       </c>
       <c r="B301" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C301" s="8" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D301" s="7" t="s">
         <v>28</v>
@@ -13872,7 +13891,7 @@
         <v>1</v>
       </c>
       <c r="H301" s="16" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="M301" s="9" t="str" cm="1">
         <f t="array" ref="M301">PAGE_NAME(B301)</f>
@@ -13888,10 +13907,10 @@
         <v>302</v>
       </c>
       <c r="B302" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C302" s="8" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D302" s="7" t="s">
         <v>28</v>
@@ -13903,7 +13922,7 @@
         <v>1</v>
       </c>
       <c r="H302" s="16" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="M302" s="9" t="str" cm="1">
         <f t="array" ref="M302">PAGE_NAME(B302)</f>
@@ -13919,10 +13938,10 @@
         <v>303</v>
       </c>
       <c r="B303" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C303" s="8" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D303" s="7" t="s">
         <v>28</v>
@@ -13947,10 +13966,10 @@
         <v>304</v>
       </c>
       <c r="B304" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C304" s="8" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="D304" s="7" t="s">
         <v>55</v>
@@ -13975,10 +13994,10 @@
         <v>305</v>
       </c>
       <c r="B305" s="11" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C305" s="8" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D305" s="7" t="s">
         <v>28</v>
@@ -13990,7 +14009,7 @@
         <v>1</v>
       </c>
       <c r="H305" s="16" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="M305" s="9" t="str" cm="1">
         <f t="array" ref="M305">PAGE_NAME(B305)</f>
@@ -14006,10 +14025,10 @@
         <v>306</v>
       </c>
       <c r="B306" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C306" s="8" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D306" s="7" t="s">
         <v>28</v>
@@ -14021,7 +14040,7 @@
         <v>1</v>
       </c>
       <c r="H306" s="16" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="307" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -14029,10 +14048,10 @@
         <v>307</v>
       </c>
       <c r="B307" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C307" s="8" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D307" s="7" t="s">
         <v>52</v>
@@ -14044,7 +14063,7 @@
         <v>1</v>
       </c>
       <c r="H307" s="16" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="M307" s="9" t="str" cm="1">
         <f t="array" ref="M307">PAGE_NAME(B307)</f>
@@ -14060,10 +14079,10 @@
         <v>308</v>
       </c>
       <c r="B308" s="11" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C308" s="8" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D308" s="7" t="s">
         <v>28</v>
@@ -14088,10 +14107,10 @@
         <v>309</v>
       </c>
       <c r="B309" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C309" s="8" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D309" s="7" t="s">
         <v>28</v>
@@ -14116,10 +14135,10 @@
         <v>310</v>
       </c>
       <c r="B310" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C310" s="8" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D310" s="7" t="s">
         <v>28</v>
@@ -14144,10 +14163,10 @@
         <v>311</v>
       </c>
       <c r="B311" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C311" s="8" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D311" s="7" t="s">
         <v>28</v>
@@ -14172,10 +14191,10 @@
         <v>312</v>
       </c>
       <c r="B312" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C312" s="8" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="D312" s="7" t="s">
         <v>28</v>
@@ -14200,10 +14219,10 @@
         <v>313</v>
       </c>
       <c r="B313" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C313" s="8" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="D313" s="7" t="s">
         <v>28</v>
@@ -14228,10 +14247,10 @@
         <v>314</v>
       </c>
       <c r="B314" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C314" s="8" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D314" s="7" t="s">
         <v>55</v>
@@ -14256,10 +14275,10 @@
         <v>315</v>
       </c>
       <c r="B315" s="11" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C315" s="8" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="D315" s="7" t="s">
         <v>28</v>
@@ -14271,7 +14290,7 @@
         <v>1</v>
       </c>
       <c r="H315" s="16" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="M315" s="9" t="str" cm="1">
         <f t="array" ref="M315">PAGE_NAME(B315)</f>
@@ -14287,10 +14306,10 @@
         <v>316</v>
       </c>
       <c r="B316" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C316" s="8" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D316" s="7" t="s">
         <v>28</v>
@@ -14302,7 +14321,7 @@
         <v>1</v>
       </c>
       <c r="H316" s="16" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="M316" s="9" t="str" cm="1">
         <f t="array" ref="M316">PAGE_NAME(B316)</f>
@@ -14318,10 +14337,10 @@
         <v>317</v>
       </c>
       <c r="B317" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C317" s="8" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D317" s="7" t="s">
         <v>28</v>
@@ -14346,10 +14365,10 @@
         <v>318</v>
       </c>
       <c r="B318" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C318" s="8" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D318" s="7" t="s">
         <v>55</v>
@@ -14374,10 +14393,10 @@
         <v>319</v>
       </c>
       <c r="B319" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C319" s="8" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D319" s="7" t="s">
         <v>55</v>
@@ -14402,10 +14421,10 @@
         <v>320</v>
       </c>
       <c r="B320" s="11" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C320" s="8" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D320" s="7" t="s">
         <v>28</v>
@@ -14430,10 +14449,10 @@
         <v>321</v>
       </c>
       <c r="B321" s="11" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C321" s="8" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="D321" s="7" t="s">
         <v>28</v>
@@ -14458,10 +14477,10 @@
         <v>322</v>
       </c>
       <c r="B322" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C322" s="8" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D322" s="7" t="s">
         <v>28</v>
@@ -14486,10 +14505,10 @@
         <v>323</v>
       </c>
       <c r="B323" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C323" s="8" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D323" s="7" t="s">
         <v>28</v>
@@ -14514,10 +14533,10 @@
         <v>324</v>
       </c>
       <c r="B324" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C324" s="8" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D324" s="7" t="s">
         <v>55</v>
@@ -14542,10 +14561,10 @@
         <v>325</v>
       </c>
       <c r="B325" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C325" s="8" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D325" s="7" t="s">
         <v>55</v>
@@ -14570,10 +14589,10 @@
         <v>326</v>
       </c>
       <c r="B326" s="7" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C326" s="8" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="D326" s="7" t="s">
         <v>52</v>
@@ -14598,10 +14617,10 @@
         <v>327</v>
       </c>
       <c r="B327" s="11" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C327" s="8" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D327" s="7" t="s">
         <v>28</v>
@@ -14613,7 +14632,7 @@
         <v>1</v>
       </c>
       <c r="H327" s="16" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="M327" s="9" t="str" cm="1">
         <f t="array" ref="M327">PAGE_NAME(B327)</f>
@@ -14629,10 +14648,10 @@
         <v>328</v>
       </c>
       <c r="B328" s="11" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C328" s="8" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D328" s="7" t="s">
         <v>52</v>
@@ -14650,7 +14669,7 @@
         <v>31</v>
       </c>
       <c r="L328" s="30" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="M328" s="9" t="str" cm="1">
         <f t="array" ref="M328">PAGE_NAME(B328)</f>
@@ -14666,10 +14685,10 @@
         <v>329</v>
       </c>
       <c r="B329" s="7" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C329" s="8" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D329" s="7" t="s">
         <v>52</v>
@@ -14687,7 +14706,7 @@
         <v>31</v>
       </c>
       <c r="L329" s="30" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="M329" s="9" t="str" cm="1">
         <f t="array" ref="M329">PAGE_NAME(B329)</f>
@@ -14703,10 +14722,10 @@
         <v>330</v>
       </c>
       <c r="B330" s="11" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C330" s="8" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D330" s="7" t="s">
         <v>52</v>
@@ -14731,10 +14750,10 @@
         <v>331</v>
       </c>
       <c r="B331" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C331" s="8" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="D331" s="7" t="s">
         <v>28</v>
@@ -14760,7 +14779,7 @@
         <v/>
       </c>
       <c r="T331" s="16" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="332" spans="1:20" ht="102" x14ac:dyDescent="0.2">
@@ -14768,10 +14787,10 @@
         <v>332</v>
       </c>
       <c r="B332" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C332" s="8" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D332" s="7" t="s">
         <v>28</v>
@@ -14802,10 +14821,10 @@
         <v>333</v>
       </c>
       <c r="B333" s="11" t="s">
+        <v>503</v>
+      </c>
+      <c r="C333" s="8" t="s">
         <v>506</v>
-      </c>
-      <c r="C333" s="8" t="s">
-        <v>509</v>
       </c>
       <c r="D333" s="7" t="s">
         <v>28</v>
@@ -14836,10 +14855,10 @@
         <v>334</v>
       </c>
       <c r="B334" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C334" s="8" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D334" s="7" t="s">
         <v>28</v>
@@ -14870,10 +14889,10 @@
         <v>335</v>
       </c>
       <c r="B335" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C335" s="8" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="D335" s="7" t="s">
         <v>28</v>
@@ -14899,7 +14918,7 @@
         <v/>
       </c>
       <c r="T335" s="16" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="336" spans="1:20" ht="102" x14ac:dyDescent="0.2">
@@ -14907,10 +14926,10 @@
         <v>336</v>
       </c>
       <c r="B336" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C336" s="8" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="D336" s="7" t="s">
         <v>28</v>
@@ -14941,10 +14960,10 @@
         <v>337</v>
       </c>
       <c r="B337" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C337" s="8" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D337" s="7" t="s">
         <v>28</v>
@@ -14969,10 +14988,10 @@
         <v>338</v>
       </c>
       <c r="B338" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C338" s="8" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D338" s="7" t="s">
         <v>104</v>
@@ -14997,10 +15016,10 @@
         <v>339</v>
       </c>
       <c r="B339" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C339" s="8" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D339" s="7" t="s">
         <v>52</v>
@@ -15034,10 +15053,10 @@
         <v>340</v>
       </c>
       <c r="B340" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C340" s="8" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D340" s="7" t="s">
         <v>52</v>
@@ -15062,10 +15081,10 @@
         <v>341</v>
       </c>
       <c r="B341" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C341" s="8" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D341" s="7" t="s">
         <v>52</v>
@@ -15080,7 +15099,7 @@
         <v>31</v>
       </c>
       <c r="J341" s="30" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="M341" s="9" t="str" cm="1">
         <f t="array" ref="M341">PAGE_NAME(B341)</f>
@@ -15096,10 +15115,10 @@
         <v>342</v>
       </c>
       <c r="B342" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C342" s="8" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="D342" s="7" t="s">
         <v>28</v>
@@ -15130,10 +15149,10 @@
         <v>343</v>
       </c>
       <c r="B343" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C343" s="8" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D343" s="7" t="s">
         <v>28</v>
@@ -15158,10 +15177,10 @@
         <v>344</v>
       </c>
       <c r="B344" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C344" s="8" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="D344" s="7" t="s">
         <v>52</v>
@@ -15186,10 +15205,10 @@
         <v>345</v>
       </c>
       <c r="B345" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C345" s="8" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D345" s="7" t="s">
         <v>55</v>
@@ -15214,10 +15233,10 @@
         <v>346</v>
       </c>
       <c r="B346" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C346" s="8" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D346" s="7" t="s">
         <v>104</v>
@@ -15229,7 +15248,7 @@
         <v>1</v>
       </c>
       <c r="H346" s="16" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="M346" s="9" t="str" cm="1">
         <f t="array" ref="M346">PAGE_NAME(B346)</f>
@@ -15245,10 +15264,10 @@
         <v>347</v>
       </c>
       <c r="B347" s="11" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C347" s="8" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D347" s="7" t="s">
         <v>28</v>
@@ -15257,7 +15276,7 @@
         <v>37</v>
       </c>
       <c r="F347" s="40" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="G347" s="7" t="b">
         <v>0</v>
@@ -15271,7 +15290,7 @@
         <v>general-considerations</v>
       </c>
       <c r="T347" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="348" spans="1:20" ht="170" x14ac:dyDescent="0.2">
@@ -15279,10 +15298,10 @@
         <v>348</v>
       </c>
       <c r="B348" s="11" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C348" s="8" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D348" s="7" t="s">
         <v>28</v>
@@ -15291,7 +15310,7 @@
         <v>56</v>
       </c>
       <c r="F348" s="8" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="G348" s="7" t="b">
         <v>0</v>
@@ -15305,7 +15324,7 @@
         <v>general-considerations</v>
       </c>
       <c r="T348" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="349" spans="1:20" ht="170" x14ac:dyDescent="0.2">
@@ -15313,10 +15332,10 @@
         <v>349</v>
       </c>
       <c r="B349" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="C349" s="8" t="s">
         <v>525</v>
-      </c>
-      <c r="C349" s="8" t="s">
-        <v>528</v>
       </c>
       <c r="D349" s="7" t="s">
         <v>28</v>
@@ -15325,13 +15344,13 @@
         <v>37</v>
       </c>
       <c r="F349" s="40" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="G349" s="7" t="b">
         <v>0</v>
       </c>
       <c r="T349" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="350" spans="1:20" ht="170" x14ac:dyDescent="0.2">
@@ -15339,10 +15358,10 @@
         <v>350</v>
       </c>
       <c r="B350" s="11" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C350" s="8" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D350" s="7" t="s">
         <v>28</v>
@@ -15351,13 +15370,13 @@
         <v>56</v>
       </c>
       <c r="F350" s="8" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="G350" s="7" t="b">
         <v>0</v>
       </c>
       <c r="T350" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="351" spans="1:20" ht="153" x14ac:dyDescent="0.2">
@@ -15365,10 +15384,10 @@
         <v>351</v>
       </c>
       <c r="B351" s="11" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C351" s="8" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="D351" s="7" t="s">
         <v>28</v>
@@ -15377,13 +15396,13 @@
         <v>37</v>
       </c>
       <c r="F351" s="40" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="G351" s="7" t="b">
         <v>0</v>
       </c>
       <c r="T351" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="352" spans="1:20" ht="153" x14ac:dyDescent="0.2">
@@ -15391,10 +15410,10 @@
         <v>352</v>
       </c>
       <c r="B352" s="11" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C352" s="8" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="D352" s="7" t="s">
         <v>28</v>
@@ -15403,13 +15422,13 @@
         <v>56</v>
       </c>
       <c r="F352" s="8" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="G352" s="7" t="b">
         <v>0</v>
       </c>
       <c r="T352" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="353" spans="1:20" ht="170" x14ac:dyDescent="0.2">
@@ -15417,16 +15436,16 @@
         <v>353</v>
       </c>
       <c r="B353" s="11" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C353" s="8" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D353" s="7" t="s">
         <v>208</v>
       </c>
       <c r="E353" s="8" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="G353" s="7" t="b">
         <v>0</v>
@@ -15440,7 +15459,7 @@
         <v>general-considerations</v>
       </c>
       <c r="T353" s="16" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="354" spans="1:20" ht="170" x14ac:dyDescent="0.2">
@@ -15448,10 +15467,10 @@
         <v>354</v>
       </c>
       <c r="B354" s="11" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C354" s="8" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D354" s="7" t="s">
         <v>208</v>
@@ -15471,7 +15490,7 @@
         <v>general-considerations</v>
       </c>
       <c r="T354" s="16" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="355" spans="1:20" ht="170" x14ac:dyDescent="0.2">
@@ -15479,10 +15498,10 @@
         <v>355</v>
       </c>
       <c r="B355" s="11" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C355" s="8" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="D355" s="7" t="s">
         <v>28</v>
@@ -15491,7 +15510,7 @@
         <v>29</v>
       </c>
       <c r="F355" s="8" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="G355" s="7" t="b">
         <v>0</v>
@@ -15505,7 +15524,7 @@
         <v>general-considerations</v>
       </c>
       <c r="T355" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="356" spans="1:20" ht="170" x14ac:dyDescent="0.2">
@@ -15513,10 +15532,10 @@
         <v>356</v>
       </c>
       <c r="B356" s="11" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C356" s="8" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="D356" s="7" t="s">
         <v>28</v>
@@ -15525,7 +15544,7 @@
         <v>29</v>
       </c>
       <c r="F356" s="40" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="G356" s="7" t="b">
         <v>0</v>
@@ -15539,7 +15558,7 @@
         <v>general-considerations</v>
       </c>
       <c r="T356" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="357" spans="1:20" ht="204" x14ac:dyDescent="0.2">
@@ -15547,10 +15566,10 @@
         <v>357</v>
       </c>
       <c r="B357" s="11" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C357" s="8" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="D357" s="7" t="s">
         <v>28</v>
@@ -15559,7 +15578,7 @@
         <v>35</v>
       </c>
       <c r="F357" s="8" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="G357" s="7" t="b">
         <v>0</v>
@@ -15573,7 +15592,7 @@
         <v>general-considerations</v>
       </c>
       <c r="T357" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="358" spans="1:20" ht="204" x14ac:dyDescent="0.2">
@@ -15581,10 +15600,10 @@
         <v>358</v>
       </c>
       <c r="B358" s="11" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C358" s="8" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="D358" s="7" t="s">
         <v>28</v>
@@ -15593,7 +15612,7 @@
         <v>35</v>
       </c>
       <c r="F358" s="40" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="G358" s="7" t="b">
         <v>0</v>
@@ -15607,7 +15626,7 @@
         <v>general-considerations</v>
       </c>
       <c r="T358" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="359" spans="1:20" ht="34" x14ac:dyDescent="0.2">
@@ -15618,7 +15637,7 @@
         <v>344</v>
       </c>
       <c r="C359" s="8" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="D359" s="7" t="s">
         <v>28</v>
@@ -15649,7 +15668,7 @@
         <v>344</v>
       </c>
       <c r="C360" s="8" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="D360" s="7" t="s">
         <v>28</v>
@@ -15674,16 +15693,16 @@
         <v>361</v>
       </c>
       <c r="B361" s="11" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C361" s="8" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="D361" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E361" s="8" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="F361" s="8"/>
       <c r="G361" s="8" t="b">
@@ -15708,7 +15727,7 @@
       <c r="R361" s="16"/>
       <c r="S361" s="16"/>
       <c r="T361" s="16" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="362" spans="1:20" s="12" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -15716,23 +15735,23 @@
         <v>362</v>
       </c>
       <c r="B362" s="11" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C362" s="8" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="D362" s="8" t="s">
         <v>55</v>
       </c>
       <c r="E362" s="8" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="F362" s="8"/>
       <c r="G362" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H362" s="16" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="I362" s="30"/>
       <c r="J362" s="30"/>
@@ -15752,7 +15771,7 @@
       <c r="R362" s="16"/>
       <c r="S362" s="16"/>
       <c r="T362" s="16" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="363" spans="1:20" s="12" customFormat="1" ht="102" x14ac:dyDescent="0.2">
@@ -15760,16 +15779,16 @@
         <v>363</v>
       </c>
       <c r="B363" s="11" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C363" s="8" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="D363" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E363" s="8" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="F363" s="8"/>
       <c r="G363" s="8" t="b">
@@ -15794,7 +15813,7 @@
       <c r="R363" s="16"/>
       <c r="S363" s="16"/>
       <c r="T363" s="16" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="364" spans="1:20" s="12" customFormat="1" ht="102" x14ac:dyDescent="0.2">
@@ -15802,23 +15821,23 @@
         <v>364</v>
       </c>
       <c r="B364" s="11" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C364" s="8" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="D364" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E364" s="8" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="F364" s="8"/>
       <c r="G364" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H364" s="16" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="I364" s="30"/>
       <c r="J364" s="30"/>
@@ -15838,7 +15857,7 @@
       <c r="R364" s="16"/>
       <c r="S364" s="16"/>
       <c r="T364" s="16" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="365" spans="1:20" s="12" customFormat="1" ht="255" x14ac:dyDescent="0.2">
@@ -15846,23 +15865,23 @@
         <v>365</v>
       </c>
       <c r="B365" s="11" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C365" s="8" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D365" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E365" s="8" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="F365" s="8"/>
       <c r="G365" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H365" s="16" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="I365" s="30"/>
       <c r="J365" s="30"/>
@@ -15882,7 +15901,7 @@
       <c r="R365" s="16"/>
       <c r="S365" s="16"/>
       <c r="T365" s="16" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="366" spans="1:20" s="12" customFormat="1" ht="119" x14ac:dyDescent="0.2">
@@ -15890,23 +15909,23 @@
         <v>366</v>
       </c>
       <c r="B366" s="11" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C366" s="8" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="D366" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E366" s="8" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="F366" s="8"/>
       <c r="G366" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H366" s="16" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="I366" s="30"/>
       <c r="J366" s="30"/>
@@ -15926,7 +15945,7 @@
       <c r="R366" s="16"/>
       <c r="S366" s="16"/>
       <c r="T366" s="16" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="367" spans="1:20" s="12" customFormat="1" ht="153" x14ac:dyDescent="0.2">
@@ -15934,23 +15953,23 @@
         <v>367</v>
       </c>
       <c r="B367" s="11" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C367" s="8" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="D367" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E367" s="8" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="F367" s="8"/>
       <c r="G367" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H367" s="16" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="I367" s="30"/>
       <c r="J367" s="30"/>
@@ -15970,7 +15989,7 @@
       <c r="R367" s="16"/>
       <c r="S367" s="16"/>
       <c r="T367" s="16" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="368" spans="1:20" s="12" customFormat="1" ht="119" x14ac:dyDescent="0.2">
@@ -15978,23 +15997,23 @@
         <v>368</v>
       </c>
       <c r="B368" s="11" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C368" s="8" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D368" s="8" t="s">
         <v>28</v>
       </c>
       <c r="E368" s="8" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="F368" s="8"/>
       <c r="G368" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H368" s="16" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="I368" s="30"/>
       <c r="J368" s="30"/>
@@ -16014,7 +16033,7 @@
       <c r="R368" s="16"/>
       <c r="S368" s="16"/>
       <c r="T368" s="16" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="369" spans="1:20" s="12" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -16022,16 +16041,16 @@
         <v>369</v>
       </c>
       <c r="B369" s="11" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C369" s="8" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="D369" s="8" t="s">
         <v>55</v>
       </c>
       <c r="E369" s="8" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="F369" s="8"/>
       <c r="G369" s="8" t="b">
@@ -16056,7 +16075,7 @@
       <c r="R369" s="16"/>
       <c r="S369" s="16"/>
       <c r="T369" s="16" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="370" spans="1:20" s="12" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -16064,23 +16083,23 @@
         <v>370</v>
       </c>
       <c r="B370" s="11" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C370" s="8" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D370" s="8" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="E370" s="8" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="F370" s="8"/>
       <c r="G370" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H370" s="16" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="I370" s="30"/>
       <c r="J370" s="30"/>
@@ -16100,7 +16119,7 @@
       <c r="R370" s="16"/>
       <c r="S370" s="16"/>
       <c r="T370" s="16" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="371" spans="1:20" s="12" customFormat="1" ht="85" x14ac:dyDescent="0.2">
@@ -16108,23 +16127,23 @@
         <v>371</v>
       </c>
       <c r="B371" s="11" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C371" s="8" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D371" s="8" t="s">
         <v>52</v>
       </c>
       <c r="E371" s="8" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="F371" s="8"/>
       <c r="G371" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H371" s="16" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="I371" s="30"/>
       <c r="J371" s="30"/>
@@ -16144,7 +16163,7 @@
       <c r="R371" s="16"/>
       <c r="S371" s="16"/>
       <c r="T371" s="16" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="372" spans="1:20" s="12" customFormat="1" ht="136" x14ac:dyDescent="0.2">
@@ -16152,23 +16171,23 @@
         <v>372</v>
       </c>
       <c r="B372" s="11" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C372" s="8" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D372" s="8" t="s">
         <v>52</v>
       </c>
       <c r="E372" s="8" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="F372" s="8"/>
       <c r="G372" s="8" t="b">
         <v>1</v>
       </c>
       <c r="H372" s="16" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="I372" s="30"/>
       <c r="J372" s="30"/>
@@ -16188,7 +16207,7 @@
       <c r="R372" s="16"/>
       <c r="S372" s="16"/>
       <c r="T372" s="16" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="373" spans="1:20" ht="16" x14ac:dyDescent="0.2">
@@ -17422,73 +17441,74 @@
     <hyperlink ref="B239" r:id="rId185" location="behavior" xr:uid="{F02E6F24-86BF-D940-9CC9-88291CE68845}"/>
     <hyperlink ref="B240" r:id="rId186" location="behavior" xr:uid="{648EFA8D-FB3D-D646-9C9C-522B4B56BAF9}"/>
     <hyperlink ref="B241" r:id="rId187" location="behavior" xr:uid="{BC5B08BD-59B1-AF4B-A285-7F01CD50D9F8}"/>
-    <hyperlink ref="B242" r:id="rId188" location="behavior" xr:uid="{B651E547-9BF9-9943-B308-F8DBD374F84C}"/>
-    <hyperlink ref="B243" r:id="rId189" location="behavior" xr:uid="{A5143A30-65E8-A542-B649-975F6CD95857}"/>
-    <hyperlink ref="B244" r:id="rId190" location="behavior" xr:uid="{D3BF5261-92C5-0446-A488-2BDE02F9809F}"/>
-    <hyperlink ref="B245" r:id="rId191" xr:uid="{80107989-1003-EC46-9A8B-283C48AAE5E2}"/>
-    <hyperlink ref="B246:B260" r:id="rId192" display="https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-dtr-smart-client.html" xr:uid="{44D2FF03-87EE-3E43-98BD-6894DF220BD4}"/>
-    <hyperlink ref="B262" r:id="rId193" location="behavior" xr:uid="{94B3AC2E-8C69-CD4E-9335-2D242398810D}"/>
-    <hyperlink ref="B263:B264" r:id="rId194" location="behavior" display="https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-full-dtr-ehr.html#behavior" xr:uid="{4CE8E25F-9A09-034D-BAD7-580DFEC4DB78}"/>
-    <hyperlink ref="B261" r:id="rId195" xr:uid="{B615E68A-EE00-644B-AC4D-A8ADC6954549}"/>
-    <hyperlink ref="B282" r:id="rId196" xr:uid="{083DBA67-8C5F-0C4D-9FEE-58A46D743032}"/>
-    <hyperlink ref="B328" r:id="rId197" xr:uid="{20C4791C-6EE8-4243-BA64-1B18365D8FDB}"/>
-    <hyperlink ref="B330" r:id="rId198" xr:uid="{AD621D40-6775-A34C-AF8B-7C8799304D40}"/>
-    <hyperlink ref="B22" r:id="rId199" location="configuring-appehr-to-payer-connectivity" xr:uid="{C77107FA-4D1F-8740-94D7-64860F4E7A6B}"/>
-    <hyperlink ref="B71" r:id="rId200" location="questionnaire-design" xr:uid="{840FB951-0207-6D4E-954E-3BAA1492471D}"/>
-    <hyperlink ref="B96" r:id="rId201" location="cql-constraints" xr:uid="{84C559FD-7957-4F44-834F-984CC40CA6BE}"/>
-    <hyperlink ref="B102" r:id="rId202" location="cql-constraints" xr:uid="{19F2A9D7-A115-424D-A6EF-2C61686438E3}"/>
-    <hyperlink ref="B168" r:id="rId203" location="retrieving-questionnaire-packages" xr:uid="{4FDB34AA-577A-FF46-94C4-9014AA0F1048}"/>
-    <hyperlink ref="B5" r:id="rId204" location="must-support" xr:uid="{793A9C56-7596-B140-986B-30D5E32C4F9C}"/>
-    <hyperlink ref="B7" r:id="rId205" location="must-support" xr:uid="{E30956E5-B1B5-8541-870E-87D92F51CDF5}"/>
-    <hyperlink ref="B347" r:id="rId206" location="general-considerations" xr:uid="{98D4FFA4-E0B0-AD42-9DFE-77750BDE434F}"/>
-    <hyperlink ref="B348" r:id="rId207" location="general-considerations" xr:uid="{BF805FE1-E999-C842-9AA2-10951D0424C2}"/>
-    <hyperlink ref="B349:B353" r:id="rId208" location="general-considerations" display="https://hl7.org/fhir/us/davinci-dtr/STU2/specification.html#general-considerations" xr:uid="{A5374E90-01B8-8943-BD89-3BF797955582}"/>
-    <hyperlink ref="B354" r:id="rId209" location="general-considerations" xr:uid="{80EA5286-DE3F-9240-8DEA-CF72FCD6F4A1}"/>
-    <hyperlink ref="B269" r:id="rId210" xr:uid="{C06E6C6E-501D-C741-B3D7-C4CB71FCF707}"/>
-    <hyperlink ref="B341" r:id="rId211" xr:uid="{26F61B15-DDEE-2948-A471-64350AFFFC0E}"/>
-    <hyperlink ref="B342" r:id="rId212" xr:uid="{35EE23D0-EFB3-6448-99CB-82441F07542A}"/>
-    <hyperlink ref="B331" r:id="rId213" xr:uid="{65F1CFFF-1656-3D4A-A26F-58FDE80B6F7D}"/>
-    <hyperlink ref="B332" r:id="rId214" xr:uid="{6898B65B-0B97-1943-8E37-BFD8E1266AB5}"/>
-    <hyperlink ref="B333" r:id="rId215" xr:uid="{1EFA02CA-FCC5-2E43-A6FA-1CD6A3AA47AE}"/>
-    <hyperlink ref="B334" r:id="rId216" xr:uid="{6C111104-81AA-3541-BA81-87A5D71770E2}"/>
-    <hyperlink ref="B335" r:id="rId217" xr:uid="{145EA780-2B5E-DD4E-9F91-7A62AB8AF3A9}"/>
-    <hyperlink ref="B336" r:id="rId218" xr:uid="{AFE6FC3E-1B9A-A742-826E-ED04C474BEA8}"/>
-    <hyperlink ref="B337" r:id="rId219" xr:uid="{27196A98-4E4F-4645-B129-788259D12238}"/>
-    <hyperlink ref="B338" r:id="rId220" xr:uid="{CED94AB2-87E3-CB48-97B5-56D20F159092}"/>
-    <hyperlink ref="B339" r:id="rId221" xr:uid="{01E6DCBB-FF37-014B-B256-34EE6D22FDA9}"/>
-    <hyperlink ref="B340" r:id="rId222" xr:uid="{1F726B02-5F16-6444-8B9E-D8B14AC43F93}"/>
-    <hyperlink ref="B343" r:id="rId223" xr:uid="{F3BD75C6-2871-0B40-AB10-A38E830CCC70}"/>
-    <hyperlink ref="B344" r:id="rId224" xr:uid="{A1E75BE7-BB31-A948-AE84-DF501C0356E3}"/>
-    <hyperlink ref="B345" r:id="rId225" xr:uid="{2225FC39-CBDA-1947-A059-F0503D779A36}"/>
-    <hyperlink ref="B346" r:id="rId226" xr:uid="{BBE77F79-F04F-6542-951A-7A61FD4D773D}"/>
-    <hyperlink ref="B355" r:id="rId227" location="general-considerations" xr:uid="{C802E133-66CC-BB43-B1FD-541D4F925C15}"/>
-    <hyperlink ref="B356" r:id="rId228" location="general-considerations" xr:uid="{90391985-B8F5-6341-8A47-A526A34FA5CE}"/>
-    <hyperlink ref="B357" r:id="rId229" location="general-considerations" xr:uid="{BB08C520-AF1F-2941-A80C-7891CF1E96B8}"/>
-    <hyperlink ref="B358" r:id="rId230" location="general-considerations" xr:uid="{DA4E5427-A4CC-B643-90B6-E6904C987AF7}"/>
-    <hyperlink ref="B151" r:id="rId231" location="authenticating-dtr-client-to-payer-api" xr:uid="{E1DCA6E6-C5B0-E842-B208-C288753DBB1A}"/>
-    <hyperlink ref="B180" r:id="rId232" location="retrieval-of-patient-fhir-resources-to-supply-to-cql-execution-engine" xr:uid="{D4C3A551-1438-4FDB-B2D1-174B10A80831}"/>
-    <hyperlink ref="B359" r:id="rId233" location="separating-user-provided-information-from-cql-retrieved-information" xr:uid="{EB1A2BC3-5FBD-0B49-9AE2-776D9A1C663D}"/>
-    <hyperlink ref="B360" r:id="rId234" location="separating-user-provided-information-from-cql-retrieved-information" xr:uid="{03BEB097-0123-8746-9289-7C76F2673EE7}"/>
-    <hyperlink ref="B167" r:id="rId235" location="retrieving-questionnaire-packages" xr:uid="{44068FFE-F585-4BFE-B6AD-3DAA3BD51BA8}"/>
-    <hyperlink ref="B152" r:id="rId236" location="authenticating-dtr-client-to-payer-api" xr:uid="{E7C4301A-D23B-4B1A-AD85-9A111EA3F001}"/>
-    <hyperlink ref="B284" r:id="rId237" xr:uid="{319CFDC3-AA49-4172-8AFA-853EAAE1B513}"/>
-    <hyperlink ref="B298" r:id="rId238" xr:uid="{EAD3E261-09C3-451A-AA9E-CF0A6E013D37}"/>
-    <hyperlink ref="B297" r:id="rId239" xr:uid="{8608BF89-2D1A-40E7-8D70-93CC94BC8797}"/>
-    <hyperlink ref="B305" r:id="rId240" xr:uid="{3BA1CBD6-E8DC-41AB-9268-A2EEDF4DD2D5}"/>
-    <hyperlink ref="B308" r:id="rId241" xr:uid="{E8173FB6-8C6F-438D-BD14-4BDE02F7388D}"/>
-    <hyperlink ref="B315" r:id="rId242" xr:uid="{92477BC8-F742-449E-A480-8FFD57A55A11}"/>
-    <hyperlink ref="B320" r:id="rId243" xr:uid="{1F52AB90-072E-43EC-902F-F2DDD53BCB05}"/>
-    <hyperlink ref="B321" r:id="rId244" xr:uid="{199B60D5-1C5B-49CA-A2DB-E0390F2DC5CF}"/>
-    <hyperlink ref="B170" r:id="rId245" location="retrieving-questionnaire-packages" xr:uid="{8426970F-13A9-4913-A64D-5FF8E3B50F75}"/>
-    <hyperlink ref="B285" r:id="rId246" xr:uid="{0B74EF60-3708-4436-B21D-7C428C326675}"/>
-    <hyperlink ref="B290" r:id="rId247" xr:uid="{99C8F7B3-5DF2-4BF8-8112-3EA54AE994B5}"/>
-    <hyperlink ref="B295" r:id="rId248" xr:uid="{5C782538-9577-4246-AB32-BD81C5CC01FD}"/>
-    <hyperlink ref="B296" r:id="rId249" xr:uid="{07AAF473-C180-4E91-9521-280924C8115F}"/>
-    <hyperlink ref="B327" r:id="rId250" xr:uid="{3A861B0B-C0F6-4DFE-AECC-1D90EC67F0B9}"/>
-    <hyperlink ref="B361" r:id="rId251" xr:uid="{08EBF7B5-A82F-ED49-9155-46570E96D149}"/>
-    <hyperlink ref="B362:B372" r:id="rId252" display="https://hl7.org/fhir/us/davinci-hrex/STU1/conformance.html" xr:uid="{59C8B298-B17A-C14C-9913-7E4D1906750B}"/>
+    <hyperlink ref="B243" r:id="rId188" location="behavior" xr:uid="{A5143A30-65E8-A542-B649-975F6CD95857}"/>
+    <hyperlink ref="B244" r:id="rId189" location="behavior" xr:uid="{D3BF5261-92C5-0446-A488-2BDE02F9809F}"/>
+    <hyperlink ref="B245" r:id="rId190" xr:uid="{80107989-1003-EC46-9A8B-283C48AAE5E2}"/>
+    <hyperlink ref="B246:B260" r:id="rId191" display="https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-dtr-smart-client.html" xr:uid="{44D2FF03-87EE-3E43-98BD-6894DF220BD4}"/>
+    <hyperlink ref="B262" r:id="rId192" location="behavior" xr:uid="{94B3AC2E-8C69-CD4E-9335-2D242398810D}"/>
+    <hyperlink ref="B263:B264" r:id="rId193" location="behavior" display="https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-full-dtr-ehr.html#behavior" xr:uid="{4CE8E25F-9A09-034D-BAD7-580DFEC4DB78}"/>
+    <hyperlink ref="B261" r:id="rId194" xr:uid="{B615E68A-EE00-644B-AC4D-A8ADC6954549}"/>
+    <hyperlink ref="B282" r:id="rId195" xr:uid="{083DBA67-8C5F-0C4D-9FEE-58A46D743032}"/>
+    <hyperlink ref="B328" r:id="rId196" xr:uid="{20C4791C-6EE8-4243-BA64-1B18365D8FDB}"/>
+    <hyperlink ref="B330" r:id="rId197" xr:uid="{AD621D40-6775-A34C-AF8B-7C8799304D40}"/>
+    <hyperlink ref="B22" r:id="rId198" location="configuring-appehr-to-payer-connectivity" xr:uid="{C77107FA-4D1F-8740-94D7-64860F4E7A6B}"/>
+    <hyperlink ref="B71" r:id="rId199" location="questionnaire-design" xr:uid="{840FB951-0207-6D4E-954E-3BAA1492471D}"/>
+    <hyperlink ref="B96" r:id="rId200" location="cql-constraints" xr:uid="{84C559FD-7957-4F44-834F-984CC40CA6BE}"/>
+    <hyperlink ref="B102" r:id="rId201" location="cql-constraints" xr:uid="{19F2A9D7-A115-424D-A6EF-2C61686438E3}"/>
+    <hyperlink ref="B168" r:id="rId202" location="retrieving-questionnaire-packages" xr:uid="{4FDB34AA-577A-FF46-94C4-9014AA0F1048}"/>
+    <hyperlink ref="B5" r:id="rId203" location="must-support" xr:uid="{793A9C56-7596-B140-986B-30D5E32C4F9C}"/>
+    <hyperlink ref="B7" r:id="rId204" location="must-support" xr:uid="{E30956E5-B1B5-8541-870E-87D92F51CDF5}"/>
+    <hyperlink ref="B347" r:id="rId205" location="general-considerations" xr:uid="{98D4FFA4-E0B0-AD42-9DFE-77750BDE434F}"/>
+    <hyperlink ref="B348" r:id="rId206" location="general-considerations" xr:uid="{BF805FE1-E999-C842-9AA2-10951D0424C2}"/>
+    <hyperlink ref="B349:B353" r:id="rId207" location="general-considerations" display="https://hl7.org/fhir/us/davinci-dtr/STU2/specification.html#general-considerations" xr:uid="{A5374E90-01B8-8943-BD89-3BF797955582}"/>
+    <hyperlink ref="B354" r:id="rId208" location="general-considerations" xr:uid="{80EA5286-DE3F-9240-8DEA-CF72FCD6F4A1}"/>
+    <hyperlink ref="B269" r:id="rId209" xr:uid="{C06E6C6E-501D-C741-B3D7-C4CB71FCF707}"/>
+    <hyperlink ref="B341" r:id="rId210" xr:uid="{26F61B15-DDEE-2948-A471-64350AFFFC0E}"/>
+    <hyperlink ref="B342" r:id="rId211" xr:uid="{35EE23D0-EFB3-6448-99CB-82441F07542A}"/>
+    <hyperlink ref="B331" r:id="rId212" xr:uid="{65F1CFFF-1656-3D4A-A26F-58FDE80B6F7D}"/>
+    <hyperlink ref="B332" r:id="rId213" xr:uid="{6898B65B-0B97-1943-8E37-BFD8E1266AB5}"/>
+    <hyperlink ref="B333" r:id="rId214" xr:uid="{1EFA02CA-FCC5-2E43-A6FA-1CD6A3AA47AE}"/>
+    <hyperlink ref="B334" r:id="rId215" xr:uid="{6C111104-81AA-3541-BA81-87A5D71770E2}"/>
+    <hyperlink ref="B335" r:id="rId216" xr:uid="{145EA780-2B5E-DD4E-9F91-7A62AB8AF3A9}"/>
+    <hyperlink ref="B336" r:id="rId217" xr:uid="{AFE6FC3E-1B9A-A742-826E-ED04C474BEA8}"/>
+    <hyperlink ref="B337" r:id="rId218" xr:uid="{27196A98-4E4F-4645-B129-788259D12238}"/>
+    <hyperlink ref="B338" r:id="rId219" xr:uid="{CED94AB2-87E3-CB48-97B5-56D20F159092}"/>
+    <hyperlink ref="B339" r:id="rId220" xr:uid="{01E6DCBB-FF37-014B-B256-34EE6D22FDA9}"/>
+    <hyperlink ref="B340" r:id="rId221" xr:uid="{1F726B02-5F16-6444-8B9E-D8B14AC43F93}"/>
+    <hyperlink ref="B343" r:id="rId222" xr:uid="{F3BD75C6-2871-0B40-AB10-A38E830CCC70}"/>
+    <hyperlink ref="B344" r:id="rId223" xr:uid="{A1E75BE7-BB31-A948-AE84-DF501C0356E3}"/>
+    <hyperlink ref="B345" r:id="rId224" xr:uid="{2225FC39-CBDA-1947-A059-F0503D779A36}"/>
+    <hyperlink ref="B346" r:id="rId225" xr:uid="{BBE77F79-F04F-6542-951A-7A61FD4D773D}"/>
+    <hyperlink ref="B355" r:id="rId226" location="general-considerations" xr:uid="{C802E133-66CC-BB43-B1FD-541D4F925C15}"/>
+    <hyperlink ref="B356" r:id="rId227" location="general-considerations" xr:uid="{90391985-B8F5-6341-8A47-A526A34FA5CE}"/>
+    <hyperlink ref="B357" r:id="rId228" location="general-considerations" xr:uid="{BB08C520-AF1F-2941-A80C-7891CF1E96B8}"/>
+    <hyperlink ref="B358" r:id="rId229" location="general-considerations" xr:uid="{DA4E5427-A4CC-B643-90B6-E6904C987AF7}"/>
+    <hyperlink ref="B151" r:id="rId230" location="authenticating-dtr-client-to-payer-api" xr:uid="{E1DCA6E6-C5B0-E842-B208-C288753DBB1A}"/>
+    <hyperlink ref="B180" r:id="rId231" location="retrieval-of-patient-fhir-resources-to-supply-to-cql-execution-engine" xr:uid="{D4C3A551-1438-4FDB-B2D1-174B10A80831}"/>
+    <hyperlink ref="B359" r:id="rId232" location="separating-user-provided-information-from-cql-retrieved-information" xr:uid="{EB1A2BC3-5FBD-0B49-9AE2-776D9A1C663D}"/>
+    <hyperlink ref="B360" r:id="rId233" location="separating-user-provided-information-from-cql-retrieved-information" xr:uid="{03BEB097-0123-8746-9289-7C76F2673EE7}"/>
+    <hyperlink ref="B167" r:id="rId234" location="retrieving-questionnaire-packages" xr:uid="{44068FFE-F585-4BFE-B6AD-3DAA3BD51BA8}"/>
+    <hyperlink ref="B152" r:id="rId235" location="authenticating-dtr-client-to-payer-api" xr:uid="{E7C4301A-D23B-4B1A-AD85-9A111EA3F001}"/>
+    <hyperlink ref="B284" r:id="rId236" xr:uid="{319CFDC3-AA49-4172-8AFA-853EAAE1B513}"/>
+    <hyperlink ref="B298" r:id="rId237" xr:uid="{EAD3E261-09C3-451A-AA9E-CF0A6E013D37}"/>
+    <hyperlink ref="B297" r:id="rId238" xr:uid="{8608BF89-2D1A-40E7-8D70-93CC94BC8797}"/>
+    <hyperlink ref="B305" r:id="rId239" xr:uid="{3BA1CBD6-E8DC-41AB-9268-A2EEDF4DD2D5}"/>
+    <hyperlink ref="B308" r:id="rId240" xr:uid="{E8173FB6-8C6F-438D-BD14-4BDE02F7388D}"/>
+    <hyperlink ref="B315" r:id="rId241" xr:uid="{92477BC8-F742-449E-A480-8FFD57A55A11}"/>
+    <hyperlink ref="B320" r:id="rId242" xr:uid="{1F52AB90-072E-43EC-902F-F2DDD53BCB05}"/>
+    <hyperlink ref="B321" r:id="rId243" xr:uid="{199B60D5-1C5B-49CA-A2DB-E0390F2DC5CF}"/>
+    <hyperlink ref="B170" r:id="rId244" location="retrieving-questionnaire-packages" xr:uid="{8426970F-13A9-4913-A64D-5FF8E3B50F75}"/>
+    <hyperlink ref="B285" r:id="rId245" xr:uid="{0B74EF60-3708-4436-B21D-7C428C326675}"/>
+    <hyperlink ref="B290" r:id="rId246" xr:uid="{99C8F7B3-5DF2-4BF8-8112-3EA54AE994B5}"/>
+    <hyperlink ref="B295" r:id="rId247" xr:uid="{5C782538-9577-4246-AB32-BD81C5CC01FD}"/>
+    <hyperlink ref="B296" r:id="rId248" xr:uid="{07AAF473-C180-4E91-9521-280924C8115F}"/>
+    <hyperlink ref="B327" r:id="rId249" xr:uid="{3A861B0B-C0F6-4DFE-AECC-1D90EC67F0B9}"/>
+    <hyperlink ref="B361" r:id="rId250" xr:uid="{08EBF7B5-A82F-ED49-9155-46570E96D149}"/>
+    <hyperlink ref="B362:B372" r:id="rId251" display="https://hl7.org/fhir/us/davinci-hrex/STU1/conformance.html" xr:uid="{59C8B298-B17A-C14C-9913-7E4D1906750B}"/>
+    <hyperlink ref="B242" r:id="rId252" location="behavior" xr:uid="{B651E547-9BF9-9943-B308-F8DBD374F84C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -17532,7 +17552,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="49" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="B1" s="49"/>
     </row>
@@ -17542,92 +17562,92 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" s="19" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="19" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
   </sheetData>
@@ -17653,19 +17673,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>558</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>559</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>560</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>561</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>562</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>563</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -17673,13 +17693,13 @@
         <v>0.1</v>
       </c>
       <c r="B2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C2" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="D2" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
   </sheetData>
@@ -17699,13 +17719,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D1" t="s">
         <v>14</v>
@@ -17719,7 +17739,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
@@ -17733,7 +17753,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="D3" t="s">
         <v>30</v>
@@ -17744,12 +17764,12 @@
         <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -18022,15 +18042,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
@@ -18041,6 +18052,15 @@
     <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18064,14 +18084,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -18087,4 +18099,12 @@
     <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix Full EHR URL in B243, B244
</commit_message>
<xml_diff>
--- a/lib/davinci_dtr_test_kit/requirements/hl7.fhir.us.davinci-dtr_2.0.1_requirements.xlsx
+++ b/lib/davinci_dtr_test_kit/requirements/hl7.fhir.us.davinci-dtr_2.0.1_requirements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knaden/Documents/Inferno/source/davinci-dtr-test-kit/lib/davinci_dtr_test_kit/requirements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstrassner/repo/inferno/davinci-dtr-test-kit/lib/davinci_dtr_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1120B00D-3D07-C844-8D02-E1B7755B7E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C4B2A0-BB3E-ED4D-A0E8-1FC0F3E63AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20380" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1994" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1994" uniqueCount="614">
   <si>
     <r>
       <rPr>
@@ -3251,9 +3251,6 @@
   </si>
   <si>
     <t>https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-full-dtr-ehr.html#behavior, https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-dtr-smart-client.html#behavior</t>
-  </si>
-  <si>
-    <t>https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-dtr-smart-client.html#behavior, https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-dtr-smart-client.html#behavior</t>
   </si>
 </sst>
 </file>
@@ -4216,10 +4213,10 @@
   <dimension ref="A1:AC476"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I238" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B245" sqref="B245"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12123,7 +12120,7 @@
         <v>243</v>
       </c>
       <c r="B243" s="11" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C243" s="8" t="s">
         <v>608</v>
@@ -12151,7 +12148,7 @@
         <v>244</v>
       </c>
       <c r="B244" s="11" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C244" s="8" t="s">
         <v>609</v>
@@ -17509,6 +17506,7 @@
     <hyperlink ref="B361" r:id="rId250" xr:uid="{08EBF7B5-A82F-ED49-9155-46570E96D149}"/>
     <hyperlink ref="B362:B372" r:id="rId251" display="https://hl7.org/fhir/us/davinci-hrex/STU1/conformance.html" xr:uid="{59C8B298-B17A-C14C-9913-7E4D1906750B}"/>
     <hyperlink ref="B242" r:id="rId252" location="behavior" display="https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-dtr-smart-client.html#behavior" xr:uid="{B651E547-9BF9-9943-B308-F8DBD374F84C}"/>
+    <hyperlink ref="B263" r:id="rId253" location="behavior" xr:uid="{B9DF0CD7-24D8-A34F-AB3D-719DB461778E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -17791,6 +17789,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -17799,7 +17810,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EC335ED7BB179244BF94A0DFE64544DC" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3a0f66abe5d2a0564332877ab55d3f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eebd8b74-b9de-41b2-9247-c010c4973c2b" xmlns:ns3="b7009bbd-f938-489b-a530-f05273710fff" xmlns:ns4="b5a44311-ed64-4a72-909f-c9dc6973bde2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ec7ca2ee893ff8a0f61d4046c6461645" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
@@ -18053,20 +18064,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="b5a44311-ed64-4a72-909f-c9dc6973bde2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Description xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-    <SortOrder xmlns="eebd8b74-b9de-41b2-9247-c010c4973c2b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
+    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
+    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA84097F-5807-4DCF-92C6-48C9EE26CFB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -18074,7 +18090,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94A9A0BE-5C9D-4319-9F23-325C29977794}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18092,22 +18108,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B0E317-5E0E-4728-AB3F-40F2C2B957FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b5a44311-ed64-4a72-909f-c9dc6973bde2"/>
-    <ds:schemaRef ds:uri="b7009bbd-f938-489b-a530-f05273710fff"/>
-    <ds:schemaRef ds:uri="eebd8b74-b9de-41b2-9247-c010c4973c2b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix requirement deprecations and multi-URL cells in spreadsheet
</commit_message>
<xml_diff>
--- a/lib/davinci_dtr_test_kit/requirements/hl7.fhir.us.davinci-dtr_2.0.1_requirements.xlsx
+++ b/lib/davinci_dtr_test_kit/requirements/hl7.fhir.us.davinci-dtr_2.0.1_requirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstrassner/repo/inferno/davinci-dtr-test-kit/lib/davinci_dtr_test_kit/requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C4B2A0-BB3E-ED4D-A0E8-1FC0F3E63AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDFC351-32CF-9F4E-9CF7-EAC638227DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20380" activeTab="1" xr2:uid="{D251129A-65BB-5042-909C-749E11B8C0B0}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -3663,7 +3663,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3766,6 +3766,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4158,14 +4159,14 @@
       <c r="C3" s="34"/>
     </row>
     <row r="4" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="45" t="s">
         <v>602</v>
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="36"/>
     </row>
     <row r="5" spans="1:3" ht="258" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="45"/>
+      <c r="A5" s="46"/>
       <c r="B5" s="39"/>
       <c r="C5" s="34"/>
     </row>
@@ -4177,17 +4178,17 @@
       <c r="C6" s="27"/>
     </row>
     <row r="7" spans="1:3" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="47"/>
+      <c r="B7" s="48"/>
     </row>
     <row r="8" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="46"/>
-      <c r="B8" s="48"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="49"/>
     </row>
     <row r="9" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="44"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="38"/>
     </row>
     <row r="10" spans="1:3" ht="292" x14ac:dyDescent="0.2">
@@ -4213,7 +4214,7 @@
   <dimension ref="A1:AC476"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
@@ -12091,7 +12092,7 @@
       <c r="A242" s="7">
         <v>242</v>
       </c>
-      <c r="B242" s="11" t="s">
+      <c r="B242" s="44" t="s">
         <v>613</v>
       </c>
       <c r="C242" s="8" t="s">
@@ -12119,7 +12120,7 @@
       <c r="A243" s="7">
         <v>243</v>
       </c>
-      <c r="B243" s="11" t="s">
+      <c r="B243" s="44" t="s">
         <v>613</v>
       </c>
       <c r="C243" s="8" t="s">
@@ -12147,7 +12148,7 @@
       <c r="A244" s="7">
         <v>244</v>
       </c>
-      <c r="B244" s="11" t="s">
+      <c r="B244" s="44" t="s">
         <v>613</v>
       </c>
       <c r="C244" s="8" t="s">
@@ -12658,7 +12659,7 @@
         <v>416</v>
       </c>
       <c r="D262" s="7" t="s">
-        <v>28</v>
+        <v>208</v>
       </c>
       <c r="E262" s="8" t="s">
         <v>66</v>
@@ -12689,7 +12690,7 @@
         <v>417</v>
       </c>
       <c r="D263" s="7" t="s">
-        <v>28</v>
+        <v>208</v>
       </c>
       <c r="E263" s="8" t="s">
         <v>66</v>
@@ -12720,7 +12721,7 @@
         <v>418</v>
       </c>
       <c r="D264" s="7" t="s">
-        <v>28</v>
+        <v>208</v>
       </c>
       <c r="E264" s="8" t="s">
         <v>66</v>
@@ -17441,72 +17442,69 @@
     <hyperlink ref="B239" r:id="rId185" location="behavior" xr:uid="{F02E6F24-86BF-D940-9CC9-88291CE68845}"/>
     <hyperlink ref="B240" r:id="rId186" location="behavior" xr:uid="{648EFA8D-FB3D-D646-9C9C-522B4B56BAF9}"/>
     <hyperlink ref="B241" r:id="rId187" location="behavior" xr:uid="{BC5B08BD-59B1-AF4B-A285-7F01CD50D9F8}"/>
-    <hyperlink ref="B243" r:id="rId188" location="behavior" display="https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-dtr-smart-client.html#behavior" xr:uid="{A5143A30-65E8-A542-B649-975F6CD95857}"/>
-    <hyperlink ref="B244" r:id="rId189" location="behavior" display="https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-dtr-smart-client.html#behavior" xr:uid="{D3BF5261-92C5-0446-A488-2BDE02F9809F}"/>
-    <hyperlink ref="B245" r:id="rId190" xr:uid="{80107989-1003-EC46-9A8B-283C48AAE5E2}"/>
-    <hyperlink ref="B246:B260" r:id="rId191" display="https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-dtr-smart-client.html" xr:uid="{44D2FF03-87EE-3E43-98BD-6894DF220BD4}"/>
-    <hyperlink ref="B262" r:id="rId192" location="behavior" xr:uid="{94B3AC2E-8C69-CD4E-9335-2D242398810D}"/>
-    <hyperlink ref="B263:B264" r:id="rId193" location="behavior" display="https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-full-dtr-ehr.html#behavior" xr:uid="{4CE8E25F-9A09-034D-BAD7-580DFEC4DB78}"/>
-    <hyperlink ref="B261" r:id="rId194" xr:uid="{B615E68A-EE00-644B-AC4D-A8ADC6954549}"/>
-    <hyperlink ref="B282" r:id="rId195" xr:uid="{083DBA67-8C5F-0C4D-9FEE-58A46D743032}"/>
-    <hyperlink ref="B328" r:id="rId196" xr:uid="{20C4791C-6EE8-4243-BA64-1B18365D8FDB}"/>
-    <hyperlink ref="B330" r:id="rId197" xr:uid="{AD621D40-6775-A34C-AF8B-7C8799304D40}"/>
-    <hyperlink ref="B22" r:id="rId198" location="configuring-appehr-to-payer-connectivity" xr:uid="{C77107FA-4D1F-8740-94D7-64860F4E7A6B}"/>
-    <hyperlink ref="B71" r:id="rId199" location="questionnaire-design" xr:uid="{840FB951-0207-6D4E-954E-3BAA1492471D}"/>
-    <hyperlink ref="B96" r:id="rId200" location="cql-constraints" xr:uid="{84C559FD-7957-4F44-834F-984CC40CA6BE}"/>
-    <hyperlink ref="B102" r:id="rId201" location="cql-constraints" xr:uid="{19F2A9D7-A115-424D-A6EF-2C61686438E3}"/>
-    <hyperlink ref="B168" r:id="rId202" location="retrieving-questionnaire-packages" xr:uid="{4FDB34AA-577A-FF46-94C4-9014AA0F1048}"/>
-    <hyperlink ref="B5" r:id="rId203" location="must-support" xr:uid="{793A9C56-7596-B140-986B-30D5E32C4F9C}"/>
-    <hyperlink ref="B7" r:id="rId204" location="must-support" xr:uid="{E30956E5-B1B5-8541-870E-87D92F51CDF5}"/>
-    <hyperlink ref="B347" r:id="rId205" location="general-considerations" xr:uid="{98D4FFA4-E0B0-AD42-9DFE-77750BDE434F}"/>
-    <hyperlink ref="B348" r:id="rId206" location="general-considerations" xr:uid="{BF805FE1-E999-C842-9AA2-10951D0424C2}"/>
-    <hyperlink ref="B349:B353" r:id="rId207" location="general-considerations" display="https://hl7.org/fhir/us/davinci-dtr/STU2/specification.html#general-considerations" xr:uid="{A5374E90-01B8-8943-BD89-3BF797955582}"/>
-    <hyperlink ref="B354" r:id="rId208" location="general-considerations" xr:uid="{80EA5286-DE3F-9240-8DEA-CF72FCD6F4A1}"/>
-    <hyperlink ref="B269" r:id="rId209" xr:uid="{C06E6C6E-501D-C741-B3D7-C4CB71FCF707}"/>
-    <hyperlink ref="B341" r:id="rId210" xr:uid="{26F61B15-DDEE-2948-A471-64350AFFFC0E}"/>
-    <hyperlink ref="B342" r:id="rId211" xr:uid="{35EE23D0-EFB3-6448-99CB-82441F07542A}"/>
-    <hyperlink ref="B331" r:id="rId212" xr:uid="{65F1CFFF-1656-3D4A-A26F-58FDE80B6F7D}"/>
-    <hyperlink ref="B332" r:id="rId213" xr:uid="{6898B65B-0B97-1943-8E37-BFD8E1266AB5}"/>
-    <hyperlink ref="B333" r:id="rId214" xr:uid="{1EFA02CA-FCC5-2E43-A6FA-1CD6A3AA47AE}"/>
-    <hyperlink ref="B334" r:id="rId215" xr:uid="{6C111104-81AA-3541-BA81-87A5D71770E2}"/>
-    <hyperlink ref="B335" r:id="rId216" xr:uid="{145EA780-2B5E-DD4E-9F91-7A62AB8AF3A9}"/>
-    <hyperlink ref="B336" r:id="rId217" xr:uid="{AFE6FC3E-1B9A-A742-826E-ED04C474BEA8}"/>
-    <hyperlink ref="B337" r:id="rId218" xr:uid="{27196A98-4E4F-4645-B129-788259D12238}"/>
-    <hyperlink ref="B338" r:id="rId219" xr:uid="{CED94AB2-87E3-CB48-97B5-56D20F159092}"/>
-    <hyperlink ref="B339" r:id="rId220" xr:uid="{01E6DCBB-FF37-014B-B256-34EE6D22FDA9}"/>
-    <hyperlink ref="B340" r:id="rId221" xr:uid="{1F726B02-5F16-6444-8B9E-D8B14AC43F93}"/>
-    <hyperlink ref="B343" r:id="rId222" xr:uid="{F3BD75C6-2871-0B40-AB10-A38E830CCC70}"/>
-    <hyperlink ref="B344" r:id="rId223" xr:uid="{A1E75BE7-BB31-A948-AE84-DF501C0356E3}"/>
-    <hyperlink ref="B345" r:id="rId224" xr:uid="{2225FC39-CBDA-1947-A059-F0503D779A36}"/>
-    <hyperlink ref="B346" r:id="rId225" xr:uid="{BBE77F79-F04F-6542-951A-7A61FD4D773D}"/>
-    <hyperlink ref="B355" r:id="rId226" location="general-considerations" xr:uid="{C802E133-66CC-BB43-B1FD-541D4F925C15}"/>
-    <hyperlink ref="B356" r:id="rId227" location="general-considerations" xr:uid="{90391985-B8F5-6341-8A47-A526A34FA5CE}"/>
-    <hyperlink ref="B357" r:id="rId228" location="general-considerations" xr:uid="{BB08C520-AF1F-2941-A80C-7891CF1E96B8}"/>
-    <hyperlink ref="B358" r:id="rId229" location="general-considerations" xr:uid="{DA4E5427-A4CC-B643-90B6-E6904C987AF7}"/>
-    <hyperlink ref="B151" r:id="rId230" location="authenticating-dtr-client-to-payer-api" xr:uid="{E1DCA6E6-C5B0-E842-B208-C288753DBB1A}"/>
-    <hyperlink ref="B180" r:id="rId231" location="retrieval-of-patient-fhir-resources-to-supply-to-cql-execution-engine" xr:uid="{D4C3A551-1438-4FDB-B2D1-174B10A80831}"/>
-    <hyperlink ref="B359" r:id="rId232" location="separating-user-provided-information-from-cql-retrieved-information" xr:uid="{EB1A2BC3-5FBD-0B49-9AE2-776D9A1C663D}"/>
-    <hyperlink ref="B360" r:id="rId233" location="separating-user-provided-information-from-cql-retrieved-information" xr:uid="{03BEB097-0123-8746-9289-7C76F2673EE7}"/>
-    <hyperlink ref="B167" r:id="rId234" location="retrieving-questionnaire-packages" xr:uid="{44068FFE-F585-4BFE-B6AD-3DAA3BD51BA8}"/>
-    <hyperlink ref="B152" r:id="rId235" location="authenticating-dtr-client-to-payer-api" xr:uid="{E7C4301A-D23B-4B1A-AD85-9A111EA3F001}"/>
-    <hyperlink ref="B284" r:id="rId236" xr:uid="{319CFDC3-AA49-4172-8AFA-853EAAE1B513}"/>
-    <hyperlink ref="B298" r:id="rId237" xr:uid="{EAD3E261-09C3-451A-AA9E-CF0A6E013D37}"/>
-    <hyperlink ref="B297" r:id="rId238" xr:uid="{8608BF89-2D1A-40E7-8D70-93CC94BC8797}"/>
-    <hyperlink ref="B305" r:id="rId239" xr:uid="{3BA1CBD6-E8DC-41AB-9268-A2EEDF4DD2D5}"/>
-    <hyperlink ref="B308" r:id="rId240" xr:uid="{E8173FB6-8C6F-438D-BD14-4BDE02F7388D}"/>
-    <hyperlink ref="B315" r:id="rId241" xr:uid="{92477BC8-F742-449E-A480-8FFD57A55A11}"/>
-    <hyperlink ref="B320" r:id="rId242" xr:uid="{1F52AB90-072E-43EC-902F-F2DDD53BCB05}"/>
-    <hyperlink ref="B321" r:id="rId243" xr:uid="{199B60D5-1C5B-49CA-A2DB-E0390F2DC5CF}"/>
-    <hyperlink ref="B170" r:id="rId244" location="retrieving-questionnaire-packages" xr:uid="{8426970F-13A9-4913-A64D-5FF8E3B50F75}"/>
-    <hyperlink ref="B285" r:id="rId245" xr:uid="{0B74EF60-3708-4436-B21D-7C428C326675}"/>
-    <hyperlink ref="B290" r:id="rId246" xr:uid="{99C8F7B3-5DF2-4BF8-8112-3EA54AE994B5}"/>
-    <hyperlink ref="B295" r:id="rId247" xr:uid="{5C782538-9577-4246-AB32-BD81C5CC01FD}"/>
-    <hyperlink ref="B296" r:id="rId248" xr:uid="{07AAF473-C180-4E91-9521-280924C8115F}"/>
-    <hyperlink ref="B327" r:id="rId249" xr:uid="{3A861B0B-C0F6-4DFE-AECC-1D90EC67F0B9}"/>
-    <hyperlink ref="B361" r:id="rId250" xr:uid="{08EBF7B5-A82F-ED49-9155-46570E96D149}"/>
-    <hyperlink ref="B362:B372" r:id="rId251" display="https://hl7.org/fhir/us/davinci-hrex/STU1/conformance.html" xr:uid="{59C8B298-B17A-C14C-9913-7E4D1906750B}"/>
-    <hyperlink ref="B242" r:id="rId252" location="behavior" display="https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-dtr-smart-client.html#behavior" xr:uid="{B651E547-9BF9-9943-B308-F8DBD374F84C}"/>
-    <hyperlink ref="B263" r:id="rId253" location="behavior" xr:uid="{B9DF0CD7-24D8-A34F-AB3D-719DB461778E}"/>
+    <hyperlink ref="B245" r:id="rId188" xr:uid="{80107989-1003-EC46-9A8B-283C48AAE5E2}"/>
+    <hyperlink ref="B246:B260" r:id="rId189" display="https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-dtr-smart-client.html" xr:uid="{44D2FF03-87EE-3E43-98BD-6894DF220BD4}"/>
+    <hyperlink ref="B262" r:id="rId190" location="behavior" xr:uid="{94B3AC2E-8C69-CD4E-9335-2D242398810D}"/>
+    <hyperlink ref="B263:B264" r:id="rId191" location="behavior" display="https://hl7.org/fhir/us/davinci-dtr/STU2/CapabilityStatement-full-dtr-ehr.html#behavior" xr:uid="{4CE8E25F-9A09-034D-BAD7-580DFEC4DB78}"/>
+    <hyperlink ref="B261" r:id="rId192" xr:uid="{B615E68A-EE00-644B-AC4D-A8ADC6954549}"/>
+    <hyperlink ref="B282" r:id="rId193" xr:uid="{083DBA67-8C5F-0C4D-9FEE-58A46D743032}"/>
+    <hyperlink ref="B328" r:id="rId194" xr:uid="{20C4791C-6EE8-4243-BA64-1B18365D8FDB}"/>
+    <hyperlink ref="B330" r:id="rId195" xr:uid="{AD621D40-6775-A34C-AF8B-7C8799304D40}"/>
+    <hyperlink ref="B22" r:id="rId196" location="configuring-appehr-to-payer-connectivity" xr:uid="{C77107FA-4D1F-8740-94D7-64860F4E7A6B}"/>
+    <hyperlink ref="B71" r:id="rId197" location="questionnaire-design" xr:uid="{840FB951-0207-6D4E-954E-3BAA1492471D}"/>
+    <hyperlink ref="B96" r:id="rId198" location="cql-constraints" xr:uid="{84C559FD-7957-4F44-834F-984CC40CA6BE}"/>
+    <hyperlink ref="B102" r:id="rId199" location="cql-constraints" xr:uid="{19F2A9D7-A115-424D-A6EF-2C61686438E3}"/>
+    <hyperlink ref="B168" r:id="rId200" location="retrieving-questionnaire-packages" xr:uid="{4FDB34AA-577A-FF46-94C4-9014AA0F1048}"/>
+    <hyperlink ref="B5" r:id="rId201" location="must-support" xr:uid="{793A9C56-7596-B140-986B-30D5E32C4F9C}"/>
+    <hyperlink ref="B7" r:id="rId202" location="must-support" xr:uid="{E30956E5-B1B5-8541-870E-87D92F51CDF5}"/>
+    <hyperlink ref="B347" r:id="rId203" location="general-considerations" xr:uid="{98D4FFA4-E0B0-AD42-9DFE-77750BDE434F}"/>
+    <hyperlink ref="B348" r:id="rId204" location="general-considerations" xr:uid="{BF805FE1-E999-C842-9AA2-10951D0424C2}"/>
+    <hyperlink ref="B349:B353" r:id="rId205" location="general-considerations" display="https://hl7.org/fhir/us/davinci-dtr/STU2/specification.html#general-considerations" xr:uid="{A5374E90-01B8-8943-BD89-3BF797955582}"/>
+    <hyperlink ref="B354" r:id="rId206" location="general-considerations" xr:uid="{80EA5286-DE3F-9240-8DEA-CF72FCD6F4A1}"/>
+    <hyperlink ref="B269" r:id="rId207" xr:uid="{C06E6C6E-501D-C741-B3D7-C4CB71FCF707}"/>
+    <hyperlink ref="B341" r:id="rId208" xr:uid="{26F61B15-DDEE-2948-A471-64350AFFFC0E}"/>
+    <hyperlink ref="B342" r:id="rId209" xr:uid="{35EE23D0-EFB3-6448-99CB-82441F07542A}"/>
+    <hyperlink ref="B331" r:id="rId210" xr:uid="{65F1CFFF-1656-3D4A-A26F-58FDE80B6F7D}"/>
+    <hyperlink ref="B332" r:id="rId211" xr:uid="{6898B65B-0B97-1943-8E37-BFD8E1266AB5}"/>
+    <hyperlink ref="B333" r:id="rId212" xr:uid="{1EFA02CA-FCC5-2E43-A6FA-1CD6A3AA47AE}"/>
+    <hyperlink ref="B334" r:id="rId213" xr:uid="{6C111104-81AA-3541-BA81-87A5D71770E2}"/>
+    <hyperlink ref="B335" r:id="rId214" xr:uid="{145EA780-2B5E-DD4E-9F91-7A62AB8AF3A9}"/>
+    <hyperlink ref="B336" r:id="rId215" xr:uid="{AFE6FC3E-1B9A-A742-826E-ED04C474BEA8}"/>
+    <hyperlink ref="B337" r:id="rId216" xr:uid="{27196A98-4E4F-4645-B129-788259D12238}"/>
+    <hyperlink ref="B338" r:id="rId217" xr:uid="{CED94AB2-87E3-CB48-97B5-56D20F159092}"/>
+    <hyperlink ref="B339" r:id="rId218" xr:uid="{01E6DCBB-FF37-014B-B256-34EE6D22FDA9}"/>
+    <hyperlink ref="B340" r:id="rId219" xr:uid="{1F726B02-5F16-6444-8B9E-D8B14AC43F93}"/>
+    <hyperlink ref="B343" r:id="rId220" xr:uid="{F3BD75C6-2871-0B40-AB10-A38E830CCC70}"/>
+    <hyperlink ref="B344" r:id="rId221" xr:uid="{A1E75BE7-BB31-A948-AE84-DF501C0356E3}"/>
+    <hyperlink ref="B345" r:id="rId222" xr:uid="{2225FC39-CBDA-1947-A059-F0503D779A36}"/>
+    <hyperlink ref="B346" r:id="rId223" xr:uid="{BBE77F79-F04F-6542-951A-7A61FD4D773D}"/>
+    <hyperlink ref="B355" r:id="rId224" location="general-considerations" xr:uid="{C802E133-66CC-BB43-B1FD-541D4F925C15}"/>
+    <hyperlink ref="B356" r:id="rId225" location="general-considerations" xr:uid="{90391985-B8F5-6341-8A47-A526A34FA5CE}"/>
+    <hyperlink ref="B357" r:id="rId226" location="general-considerations" xr:uid="{BB08C520-AF1F-2941-A80C-7891CF1E96B8}"/>
+    <hyperlink ref="B358" r:id="rId227" location="general-considerations" xr:uid="{DA4E5427-A4CC-B643-90B6-E6904C987AF7}"/>
+    <hyperlink ref="B151" r:id="rId228" location="authenticating-dtr-client-to-payer-api" xr:uid="{E1DCA6E6-C5B0-E842-B208-C288753DBB1A}"/>
+    <hyperlink ref="B180" r:id="rId229" location="retrieval-of-patient-fhir-resources-to-supply-to-cql-execution-engine" xr:uid="{D4C3A551-1438-4FDB-B2D1-174B10A80831}"/>
+    <hyperlink ref="B359" r:id="rId230" location="separating-user-provided-information-from-cql-retrieved-information" xr:uid="{EB1A2BC3-5FBD-0B49-9AE2-776D9A1C663D}"/>
+    <hyperlink ref="B360" r:id="rId231" location="separating-user-provided-information-from-cql-retrieved-information" xr:uid="{03BEB097-0123-8746-9289-7C76F2673EE7}"/>
+    <hyperlink ref="B167" r:id="rId232" location="retrieving-questionnaire-packages" xr:uid="{44068FFE-F585-4BFE-B6AD-3DAA3BD51BA8}"/>
+    <hyperlink ref="B152" r:id="rId233" location="authenticating-dtr-client-to-payer-api" xr:uid="{E7C4301A-D23B-4B1A-AD85-9A111EA3F001}"/>
+    <hyperlink ref="B284" r:id="rId234" xr:uid="{319CFDC3-AA49-4172-8AFA-853EAAE1B513}"/>
+    <hyperlink ref="B298" r:id="rId235" xr:uid="{EAD3E261-09C3-451A-AA9E-CF0A6E013D37}"/>
+    <hyperlink ref="B297" r:id="rId236" xr:uid="{8608BF89-2D1A-40E7-8D70-93CC94BC8797}"/>
+    <hyperlink ref="B305" r:id="rId237" xr:uid="{3BA1CBD6-E8DC-41AB-9268-A2EEDF4DD2D5}"/>
+    <hyperlink ref="B308" r:id="rId238" xr:uid="{E8173FB6-8C6F-438D-BD14-4BDE02F7388D}"/>
+    <hyperlink ref="B315" r:id="rId239" xr:uid="{92477BC8-F742-449E-A480-8FFD57A55A11}"/>
+    <hyperlink ref="B320" r:id="rId240" xr:uid="{1F52AB90-072E-43EC-902F-F2DDD53BCB05}"/>
+    <hyperlink ref="B321" r:id="rId241" xr:uid="{199B60D5-1C5B-49CA-A2DB-E0390F2DC5CF}"/>
+    <hyperlink ref="B170" r:id="rId242" location="retrieving-questionnaire-packages" xr:uid="{8426970F-13A9-4913-A64D-5FF8E3B50F75}"/>
+    <hyperlink ref="B285" r:id="rId243" xr:uid="{0B74EF60-3708-4436-B21D-7C428C326675}"/>
+    <hyperlink ref="B290" r:id="rId244" xr:uid="{99C8F7B3-5DF2-4BF8-8112-3EA54AE994B5}"/>
+    <hyperlink ref="B295" r:id="rId245" xr:uid="{5C782538-9577-4246-AB32-BD81C5CC01FD}"/>
+    <hyperlink ref="B296" r:id="rId246" xr:uid="{07AAF473-C180-4E91-9521-280924C8115F}"/>
+    <hyperlink ref="B327" r:id="rId247" xr:uid="{3A861B0B-C0F6-4DFE-AECC-1D90EC67F0B9}"/>
+    <hyperlink ref="B361" r:id="rId248" xr:uid="{08EBF7B5-A82F-ED49-9155-46570E96D149}"/>
+    <hyperlink ref="B362:B372" r:id="rId249" display="https://hl7.org/fhir/us/davinci-hrex/STU1/conformance.html" xr:uid="{59C8B298-B17A-C14C-9913-7E4D1906750B}"/>
+    <hyperlink ref="B263" r:id="rId250" location="behavior" xr:uid="{B9DF0CD7-24D8-A34F-AB3D-719DB461778E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -17552,14 +17550,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>603</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="50"/>
     </row>
     <row r="2" spans="1:2" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">

</xml_diff>